<commit_message>
Updated data figures titles
</commit_message>
<xml_diff>
--- a/Final Report/Experimental Data/Dynomometer vs Pressure.xlsx
+++ b/Final Report/Experimental Data/Dynomometer vs Pressure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arobo\Documents\GitHub\Hydraulic-Mimic-Arm\Final Report\Experimental Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF4E486-B556-4EFF-B1E9-B0155B2088F7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5930CEC8-D4C5-4E69-84BA-6099131B506F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7965" xr2:uid="{83A5CEDF-E666-4F4A-BF91-CC0FB8030E4B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7965" firstSheet="1" activeTab="2" xr2:uid="{83A5CEDF-E666-4F4A-BF91-CC0FB8030E4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynonometer vs Pressure" sheetId="1" r:id="rId1"/>
@@ -32,18 +32,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Dynomometer (kg)</t>
   </si>
   <si>
-    <t>Pressure(bar)</t>
-  </si>
-  <si>
     <t>pressure</t>
-  </si>
-  <si>
-    <t>force</t>
   </si>
   <si>
     <t>Cylinder Properties</t>
@@ -73,14 +67,26 @@
     <t>force (N)</t>
   </si>
   <si>
-    <t>theoretical force (N)</t>
+    <t>Pressure(MPa)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dynomometer Power Grasp </t>
+  </si>
+  <si>
+    <t>force (kg)</t>
+  </si>
+  <si>
+    <t>Force (N)</t>
+  </si>
+  <si>
+    <t>Theoretical Force (N)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,6 +96,13 @@
     </font>
     <font>
       <sz val="9"/>
+      <color rgb="FF595959"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color rgb="FF595959"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -116,9 +129,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -153,6 +169,37 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Dynomometer </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Power Grasp </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -231,25 +278,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14</c:v>
+                  <c:v>1.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>18</c:v>
+                  <c:v>1.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -323,6 +370,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Pressure (MPa)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -385,6 +487,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Dynomometer</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-AU" baseline="0"/>
+                  <a:t> (kg)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-AU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -492,6 +654,66 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>Cylinder Retraction</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-AU" baseline="0"/>
+              <a:t> Force</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-AU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -503,11 +725,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Dynonometer vs Pressure (no r)'!$B$1</c:f>
+              <c:f>'pressure vs direct cyl '!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>force</c:v>
+                  <c:v>Force (N)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -534,34 +756,814 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'pressure vs direct cyl '!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'pressure vs direct cyl '!$B$2:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>16.43</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>47.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>61.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B5B3-49A7-88C1-E29E839B1F84}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'pressure vs direct cyl '!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Theoretical Force (N)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
             <c:spPr>
-              <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'pressure vs direct cyl '!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'pressure vs direct cyl '!$C$2:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>21.161248000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31.741872000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42.322496000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>52.903120000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>63.483744000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>74.064368000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>84.644992000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>95.225616000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B5B3-49A7-88C1-E29E839B1F84}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1776969151"/>
+        <c:axId val="1779491711"/>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'pressure vs direct cyl '!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Efficiency</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="dashDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'pressure vs direct cyl '!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'pressure vs direct cyl '!$D$2:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.77641923576530081</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.75609907317375613</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.73247097713707621</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7750015500031</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.74822304116152949</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.72909553484612188</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.72892676273157431</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.75609907317375613</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B5B3-49A7-88C1-E29E839B1F84}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1867614303"/>
+        <c:axId val="1867610143"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1776969151"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Pressure (MPa)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1779491711"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1779491711"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Retraction Force (N)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1776969151"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1867610143"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:noFill/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1867614303"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1867614303"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1867610143"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>Dynomometer Power Grasp </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>(without elastic external</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-AU" baseline="0"/>
+              <a:t> extension)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-AU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Dynonometer vs Pressure (no r)'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>force (kg)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
-                <a:prstDash val="sysDot"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>'Dynonometer vs Pressure (no r)'!$A$2:$A$9</c:f>
@@ -569,43 +1571,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14</c:v>
+                  <c:v>1.4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18</c:v>
+                  <c:v>1.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Dynonometer vs Pressure (no r)'!$B$2:$B$9</c:f>
+              <c:f>'Dynonometer vs Pressure (no r)'!$D$2:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>7.75</c:v>
@@ -618,6 +1623,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -711,6 +1719,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Pressure (MPa)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -773,6 +1836,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Dynomometer</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-AU" baseline="0"/>
+                  <a:t> (kg)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-AU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -946,6 +2069,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1978,20 +3141,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2023,16 +3702,57 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>581024</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>185736</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>495299</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CFDAAF7-D098-497F-948D-3B74C57A0B3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2357,28 +4077,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8929C082-F7D1-4295-862C-786A2D8F6EE2}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>6</v>
+        <v>0.6</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -2387,77 +4107,105 @@
         <f>B2*9.82</f>
         <v>39.28</v>
       </c>
+      <c r="D2">
+        <f t="shared" ref="D2:D7" si="0">A2/10</f>
+        <v>0.06</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>8</v>
+        <v>0.8</v>
       </c>
       <c r="B3">
         <v>5.5</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C8" si="0">B3*9.82</f>
+        <f t="shared" ref="C3:C8" si="1">B3*9.82</f>
         <v>54.010000000000005</v>
       </c>
+      <c r="D3">
+        <f t="shared" si="0"/>
+        <v>0.08</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B4">
         <v>5.9</v>
       </c>
       <c r="C4">
+        <f t="shared" si="1"/>
+        <v>57.938000000000002</v>
+      </c>
+      <c r="D4">
         <f t="shared" si="0"/>
-        <v>57.938000000000002</v>
+        <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>12</v>
+        <v>1.2</v>
       </c>
       <c r="B5">
         <v>7</v>
       </c>
       <c r="C5">
+        <f t="shared" si="1"/>
+        <v>68.740000000000009</v>
+      </c>
+      <c r="D5">
         <f t="shared" si="0"/>
-        <v>68.740000000000009</v>
+        <v>0.12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>14</v>
+        <v>1.4</v>
       </c>
       <c r="B6">
         <v>8</v>
       </c>
       <c r="C6">
+        <f t="shared" si="1"/>
+        <v>78.56</v>
+      </c>
+      <c r="D6">
         <f t="shared" si="0"/>
-        <v>78.56</v>
+        <v>0.13999999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>16</v>
+        <v>1.6</v>
       </c>
       <c r="B7">
         <v>9.75</v>
       </c>
       <c r="C7">
+        <f t="shared" si="1"/>
+        <v>95.745000000000005</v>
+      </c>
+      <c r="D7">
         <f t="shared" si="0"/>
-        <v>95.745000000000005</v>
+        <v>0.16</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>18</v>
+        <v>1.8</v>
       </c>
       <c r="B8">
         <v>10.5</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>103.11</v>
+      </c>
+      <c r="D8">
+        <f>A8/10</f>
+        <v>0.18</v>
       </c>
     </row>
   </sheetData>
@@ -2471,7 +4219,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2481,44 +4229,48 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>4</v>
+        <v>0.4</v>
       </c>
       <c r="B2">
         <v>16.43</v>
       </c>
       <c r="C2">
-        <f>A2*I$4*(I$2-I$3)</f>
+        <f>A2*1000000*(I$2-I$3)</f>
         <v>21.161248000000001</v>
       </c>
       <c r="D2">
         <f>B2/C2</f>
         <v>0.77641923576530081</v>
       </c>
+      <c r="E2">
+        <f>A2/10</f>
+        <v>0.04</v>
+      </c>
       <c r="G2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H2">
         <v>0.11</v>
@@ -2530,21 +4282,25 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>6</v>
+        <v>0.6</v>
       </c>
       <c r="B3">
         <v>24</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C9" si="0">A3*I$4*(I$2-I$3)</f>
+        <f t="shared" ref="C3:C9" si="0">A3*1000000*(I$2-I$3)</f>
         <v>31.741872000000001</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D9" si="1">B3/C3</f>
         <v>0.75609907317375613</v>
       </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E9" si="2">A3/10</f>
+        <v>0.06</v>
+      </c>
       <c r="G3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H3">
         <v>2.8000000000000001E-2</v>
@@ -2556,7 +4312,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>8</v>
+        <v>0.8</v>
       </c>
       <c r="B4">
         <v>31</v>
@@ -2569,8 +4325,12 @@
         <f t="shared" si="1"/>
         <v>0.73247097713707621</v>
       </c>
+      <c r="E4">
+        <f t="shared" si="2"/>
+        <v>0.08</v>
+      </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I4">
         <v>100000</v>
@@ -2578,7 +4338,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B5">
         <v>41</v>
@@ -2591,10 +4351,14 @@
         <f t="shared" si="1"/>
         <v>0.7750015500031</v>
       </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>12</v>
+        <v>1.2</v>
       </c>
       <c r="B6">
         <v>47.5</v>
@@ -2607,10 +4371,14 @@
         <f t="shared" si="1"/>
         <v>0.74822304116152949</v>
       </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>0.12</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>14</v>
+        <v>1.4</v>
       </c>
       <c r="B7">
         <v>54</v>
@@ -2623,10 +4391,14 @@
         <f t="shared" si="1"/>
         <v>0.72909553484612188</v>
       </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>0.13999999999999999</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>16</v>
+        <v>1.6</v>
       </c>
       <c r="B8">
         <v>61.7</v>
@@ -2639,10 +4411,14 @@
         <f t="shared" si="1"/>
         <v>0.72892676273157431</v>
       </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>0.16</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>18</v>
+        <v>1.8</v>
       </c>
       <c r="B9">
         <v>72</v>
@@ -2654,6 +4430,10 @@
       <c r="D9">
         <f t="shared" si="1"/>
         <v>0.75609907317375613</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>0.18</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2670,30 +4450,31 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8053FA6-F505-435E-9AC5-03C18D67843A}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>4</v>
+        <v>0.4</v>
       </c>
       <c r="C2">
         <f>B2*9.82</f>
@@ -2706,10 +4487,14 @@
         <f>D2*9.82</f>
         <v>49.1</v>
       </c>
+      <c r="G2">
+        <f>A2/10</f>
+        <v>0.04</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>6</v>
+        <v>0.6</v>
       </c>
       <c r="B3">
         <v>6</v>
@@ -2725,10 +4510,14 @@
         <f t="shared" si="0"/>
         <v>58.92</v>
       </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G9" si="1">A3/10</f>
+        <v>0.06</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>8</v>
+        <v>0.8</v>
       </c>
       <c r="B4">
         <v>6</v>
@@ -2744,10 +4533,14 @@
         <f>D4*9.82</f>
         <v>63.83</v>
       </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>0.08</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B5">
         <v>7.75</v>
@@ -2763,10 +4556,14 @@
         <f t="shared" si="0"/>
         <v>76.105000000000004</v>
       </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>12</v>
+        <v>1.2</v>
       </c>
       <c r="B6">
         <v>9</v>
@@ -2782,10 +4579,14 @@
         <f t="shared" si="0"/>
         <v>88.38</v>
       </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>14</v>
+        <v>1.4</v>
       </c>
       <c r="B7">
         <v>10</v>
@@ -2801,10 +4602,14 @@
         <f t="shared" si="0"/>
         <v>98.2</v>
       </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>0.13999999999999999</v>
+      </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>16</v>
+        <v>1.6</v>
       </c>
       <c r="B8">
         <v>10.5</v>
@@ -2820,10 +4625,14 @@
         <f>D8*9.82</f>
         <v>103.11</v>
       </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>0.16</v>
+      </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>18</v>
+        <v>1.8</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
@@ -2835,6 +4644,15 @@
       <c r="E9">
         <f t="shared" si="0"/>
         <v>117.84</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J11" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>